<commit_message>
01_JAVA 기본 & 심화 done
</commit_message>
<xml_diff>
--- a/18회차_실습체크리스트_홍길동.xlsx
+++ b/18회차_실습체크리스트_홍길동.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\비전공_18회차\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fullstack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,50 +209,135 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>이름 : 홍길동</t>
+    <t>06 중첩 객체</t>
+  </si>
+  <si>
+    <t>07 예외처리, 라이브러리</t>
+  </si>
+  <si>
+    <t>08 멀티스레드</t>
+  </si>
+  <si>
+    <t>09 제너릭, 컬렉션</t>
+  </si>
+  <si>
+    <t>10 컬렉션</t>
+  </si>
+  <si>
+    <t>11 람다식</t>
+  </si>
+  <si>
+    <t>12 스트림 요소 처리</t>
+  </si>
+  <si>
+    <t>13 데이터 입출력</t>
+  </si>
+  <si>
+    <t>01_java(기본)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>01 개발환경 구축, 변수, 타입, 연산자</t>
-  </si>
-  <si>
-    <t>02 조건문과 반복문, 참조타입</t>
-  </si>
-  <si>
-    <t>03 클래스</t>
-  </si>
-  <si>
-    <t>04 상속</t>
-  </si>
-  <si>
-    <t>05 인터페이스</t>
-  </si>
-  <si>
-    <t>06 중첩 객체</t>
-  </si>
-  <si>
-    <t>07 예외처리, 라이브러리</t>
-  </si>
-  <si>
-    <t>08 멀티스레드</t>
-  </si>
-  <si>
-    <t>09 제너릭, 컬렉션</t>
-  </si>
-  <si>
-    <t>10 컬렉션</t>
-  </si>
-  <si>
-    <t>11 람다식</t>
-  </si>
-  <si>
-    <t>12 스트림 요소 처리</t>
-  </si>
-  <si>
-    <t>13 데이터 입출력</t>
-  </si>
-  <si>
-    <t>01_java(기본)</t>
+    <t>02_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>03_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>04_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>05_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>06_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>07_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>08_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>09_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>11_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>12_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>13_java(기본)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>12_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>01_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>02_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>03_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>04_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>05_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>06_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>07_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>08_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>09_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>11_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>13_java(심화)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>제출일자: 5월 12일(월) 23시 59분까지</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -261,107 +346,27 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>02_java(기본)</t>
+    <t>01 개발환경 구축, 변수, 타입, 연산자</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>03_java(기본)</t>
+    <t>02 조건문과 반복문, 참조타입</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>04_java(기본)</t>
+    <t>이름 : 안다윤</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>05_java(기본)</t>
+    <t>03 클래스</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>06_java(기본)</t>
+    <t>04 상속</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>07_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>08_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>09_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>10_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>11_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>12_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_java(기본)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>12_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>01_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>02_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>03_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>04_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>05_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>06_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>07_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>08_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>09_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>10_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>11_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_java(심화)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>제출일자: 5월 12일(월) 23시 59분까지</t>
+    <t>05 인터페이스</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -675,6 +680,9 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,6 +690,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -716,15 +730,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,7 +825,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
@@ -902,7 +907,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -969,7 +974,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1036,7 +1041,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1103,7 +1108,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1170,7 +1175,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1237,7 +1242,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1304,7 +1309,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193430</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1371,7 +1376,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193430</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1438,7 +1443,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1505,7 +1510,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1572,7 +1577,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1639,7 +1644,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>193431</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2108,7 +2113,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2175,7 +2180,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2242,7 +2247,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>9524</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2309,7 +2314,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>9524</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2644,7 +2649,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2711,7 +2716,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2778,7 +2783,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>9524</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2845,7 +2850,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>9524</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3607,8 +3612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3620,36 +3625,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="27" customHeight="1">
-      <c r="A3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="16" t="s">
+      <c r="A3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
@@ -3672,236 +3677,236 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="22.5">
-      <c r="A5" s="17" t="s">
-        <v>25</v>
+      <c r="A5" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="17"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="22"/>
+        <v>47</v>
+      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="22"/>
+        <v>49</v>
+      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="17"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="22"/>
+        <v>51</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="22"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="17"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="8"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="C12" s="8"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="22"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="8"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="17"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="22"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="17"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="22"/>
+        <v>15</v>
+      </c>
+      <c r="C15" s="8"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="22"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="8"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="17"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="A22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>